<commit_message>
[IMP] z0bug_odoo: test data for MtO
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/sale_order.xlsx
+++ b/z0bug_odoo/data/sale_order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">ddt_type_id</t>
   </si>
   <si>
+    <t xml:space="preserve">payment_term_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.sale_order_Z0_1</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t xml:space="preserve">l10n_it_ddt.ddt_type_ddt</t>
   </si>
   <si>
+    <t xml:space="preserve">z0bug.payment_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.sale_order_Z0_2</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.payment_2</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.sale_order_Z0_3</t>
@@ -143,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,6 +187,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +254,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,13 +282,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20"/>
@@ -267,6 +297,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,152 +322,161 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="n">
         <v>210123</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="n">
         <v>21011214</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>